<commit_message>
Refactored reroll code, added demo variable
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5BF57F-462D-4543-920A-CB7B8FF52E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25494C16-61C8-4DD9-9F96-0F02B457458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" activeTab="2" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="markers" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Blue</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Azure Blue</t>
   </si>
   <si>
-    <t>Violet Purple</t>
-  </si>
-  <si>
     <t>Grey</t>
   </si>
   <si>
@@ -149,6 +146,12 @@
   </si>
   <si>
     <t>Mid Blue</t>
+  </si>
+  <si>
+    <t>Egg Blue</t>
+  </si>
+  <si>
+    <t>Eggplant Purple</t>
   </si>
 </sst>
 </file>
@@ -585,14 +588,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FB3344-4CE2-4D30-BDA1-D2A938E8401D}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,7 +625,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -631,6 +634,9 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,15 +658,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8021D7E5-C5D3-468A-8962-5308880DA2DD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -668,39 +677,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits to comments and whitespace, added exit text
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25494C16-61C8-4DD9-9F96-0F02B457458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3CD8B4-AC75-47D2-80D5-C46F708799CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="markers" sheetId="1" r:id="rId1"/>
     <sheet name="watercolours" sheetId="3" r:id="rId2"/>
     <sheet name="paints" sheetId="4" r:id="rId3"/>
+    <sheet name="crayons" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Blue</t>
   </si>
@@ -152,16 +153,85 @@
   </si>
   <si>
     <t>Eggplant Purple</t>
+  </si>
+  <si>
+    <t>Purples</t>
+  </si>
+  <si>
+    <t>Blues</t>
+  </si>
+  <si>
+    <t>Reds</t>
+  </si>
+  <si>
+    <t>V01</t>
+  </si>
+  <si>
+    <t>V02</t>
+  </si>
+  <si>
+    <t>V03</t>
+  </si>
+  <si>
+    <t>V04</t>
+  </si>
+  <si>
+    <t>V05</t>
+  </si>
+  <si>
+    <t>V06</t>
+  </si>
+  <si>
+    <t>V07</t>
+  </si>
+  <si>
+    <t>V08</t>
+  </si>
+  <si>
+    <t>V09</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>B03</t>
+  </si>
+  <si>
+    <t>B04</t>
+  </si>
+  <si>
+    <t>B05</t>
+  </si>
+  <si>
+    <t>B06</t>
+  </si>
+  <si>
+    <t>B07</t>
+  </si>
+  <si>
+    <t>R01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -588,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FB3344-4CE2-4D30-BDA1-D2A938E8401D}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -715,4 +785,105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8200B3D-79D9-4DB0-A7F2-3CBE4D435429}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding a mode selector to customise sheet access
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3CD8B4-AC75-47D2-80D5-C46F708799CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D3566-0532-443F-9251-4DFEE3DA7712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="markers" sheetId="1" r:id="rId1"/>
     <sheet name="watercolours" sheetId="3" r:id="rId2"/>
     <sheet name="paints" sheetId="4" r:id="rId3"/>
-    <sheet name="crayons" sheetId="5" r:id="rId4"/>
+    <sheet name="personal" sheetId="5" r:id="rId4"/>
+    <sheet name="private" sheetId="9" r:id="rId5"/>
+    <sheet name="business1" sheetId="6" r:id="rId6"/>
+    <sheet name="business2" sheetId="8" r:id="rId7"/>
+    <sheet name="business3" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
   <si>
     <t>Blue</t>
   </si>
@@ -216,6 +220,69 @@
   </si>
   <si>
     <t>R01</t>
+  </si>
+  <si>
+    <t>Hex1</t>
+  </si>
+  <si>
+    <t>Hex2</t>
+  </si>
+  <si>
+    <t>Hex3</t>
+  </si>
+  <si>
+    <t>Hex6</t>
+  </si>
+  <si>
+    <t>Hex7</t>
+  </si>
+  <si>
+    <t>Hex8</t>
+  </si>
+  <si>
+    <t>Hex4</t>
+  </si>
+  <si>
+    <t>Hex5</t>
+  </si>
+  <si>
+    <t>purple02 p</t>
+  </si>
+  <si>
+    <t>purple01 p</t>
+  </si>
+  <si>
+    <t>purple03 p</t>
+  </si>
+  <si>
+    <t>purple04 p</t>
+  </si>
+  <si>
+    <t>purple05 p</t>
+  </si>
+  <si>
+    <t>blue01 p</t>
+  </si>
+  <si>
+    <t>blue02 p</t>
+  </si>
+  <si>
+    <t>blue03 p</t>
+  </si>
+  <si>
+    <t>blue04 p</t>
+  </si>
+  <si>
+    <t>blue05 p</t>
+  </si>
+  <si>
+    <t>blue06 p</t>
+  </si>
+  <si>
+    <t>blue07 p</t>
+  </si>
+  <si>
+    <t>red01 p</t>
   </si>
 </sst>
 </file>
@@ -791,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8200B3D-79D9-4DB0-A7F2-3CBE4D435429}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,4 +953,513 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B705373B-808D-4771-B708-A48EFE188BCB}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5A2C93-BD89-4B55-941F-F99B73CD3264}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(10000,99999)</f>
+        <v>46598</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="A2:C13" ca="1" si="0">RANDBETWEEN(10000,99999)</f>
+        <v>75930</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ca="1" si="0"/>
+        <v>73923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ca="1" si="0"/>
+        <v>10007</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>49073</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>19714</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>28035</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>29888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>19652</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>90003</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>63453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>19603</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>15066</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>10296</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>55608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>21279</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>70605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>65168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>69252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>66717</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>56973</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>71581</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DC0507-2589-4AC1-9862-D7928C83B4FC}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(10000,99999)</f>
+        <v>47017</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="A2:D13" ca="1" si="0">RANDBETWEEN(10000,99999)</f>
+        <v>52585</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ca="1" si="0"/>
+        <v>40692</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ca="1" si="0"/>
+        <v>28953</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>26682</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>41449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>50228</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>60962</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>48668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>81045</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>56796</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>26988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>59330</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>16757</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>76198</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>19933</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>52898</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>19022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>56839</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>14838</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>30317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>84923</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>21010</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213BADF4-84EF-4347-B750-C4FDA302935A}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(10000,99999)</f>
+        <v>11192</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="A2:D13" ca="1" si="0">RANDBETWEEN(10000,99999)</f>
+        <v>33531</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ca="1" si="0"/>
+        <v>32337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ca="1" si="0"/>
+        <v>35796</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>83056</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>70503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>32911</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>70486</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>66188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>89239</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>33323</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>72907</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>91386</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>98747</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>14283</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>50360</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>49099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>82951</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>76748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>81329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>31460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the data_clean script to process data cleansing
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D3566-0532-443F-9251-4DFEE3DA7712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B00994-A718-4C12-BD3E-2A4F811DFE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="markers" sheetId="1" r:id="rId1"/>
-    <sheet name="watercolours" sheetId="3" r:id="rId2"/>
-    <sheet name="paints" sheetId="4" r:id="rId3"/>
-    <sheet name="personal" sheetId="5" r:id="rId4"/>
-    <sheet name="private" sheetId="9" r:id="rId5"/>
-    <sheet name="business1" sheetId="6" r:id="rId6"/>
-    <sheet name="business2" sheetId="8" r:id="rId7"/>
-    <sheet name="business3" sheetId="7" r:id="rId8"/>
+    <sheet name="paints" sheetId="4" r:id="rId2"/>
+    <sheet name="personal" sheetId="5" r:id="rId3"/>
+    <sheet name="private" sheetId="9" r:id="rId4"/>
+    <sheet name="business1" sheetId="6" r:id="rId5"/>
+    <sheet name="business2" sheetId="8" r:id="rId6"/>
+    <sheet name="business3" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>Blue</t>
   </si>
@@ -96,33 +95,6 @@
     <t>Camo</t>
   </si>
   <si>
-    <t>Purple</t>
-  </si>
-  <si>
-    <t>Pastel Pink</t>
-  </si>
-  <si>
-    <t>Rose Pink</t>
-  </si>
-  <si>
-    <t>Very Pink</t>
-  </si>
-  <si>
-    <t>Rouge Pink</t>
-  </si>
-  <si>
-    <t>Royal Purple</t>
-  </si>
-  <si>
-    <t>Baby Pink</t>
-  </si>
-  <si>
-    <t>Sea Blue</t>
-  </si>
-  <si>
-    <t>Azure Blue</t>
-  </si>
-  <si>
     <t>Grey</t>
   </si>
   <si>
@@ -151,12 +123,6 @@
   </si>
   <si>
     <t>Mid Blue</t>
-  </si>
-  <si>
-    <t>Egg Blue</t>
-  </si>
-  <si>
-    <t>Eggplant Purple</t>
   </si>
   <si>
     <t>Purples</t>
@@ -722,80 +688,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FB3344-4CE2-4D30-BDA1-D2A938E8401D}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8021D7E5-C5D3-468A-8962-5308880DA2DD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -806,7 +702,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -814,39 +710,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8200B3D-79D9-4DB0-A7F2-3CBE4D435429}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -866,87 +762,87 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -955,7 +851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B705373B-808D-4771-B708-A48EFE188BCB}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -970,66 +866,66 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1038,141 +934,237 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5A2C93-BD89-4B55-941F-F99B73CD3264}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f ca="1">RANDBETWEEN(10000,99999)</f>
-        <v>46598</v>
+        <v>97275</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="A2:C13" ca="1" si="0">RANDBETWEEN(10000,99999)</f>
-        <v>75930</v>
+        <v>30853</v>
       </c>
       <c r="C2">
-        <f t="shared" ca="1" si="0"/>
-        <v>73923</v>
+        <v>66119</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ca="1" si="0"/>
-        <v>10007</v>
+        <v>19804</v>
       </c>
       <c r="B3">
-        <f t="shared" ca="1" si="0"/>
-        <v>49073</v>
+        <v>87240</v>
       </c>
       <c r="C3">
-        <f t="shared" ca="1" si="0"/>
-        <v>44112</v>
+        <v>36420</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ca="1" si="0"/>
-        <v>19714</v>
+        <v>47346</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>28035</v>
+        <v>40594</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>29888</v>
+        <v>46815</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>19652</v>
+        <v>76368</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>90003</v>
+        <v>30299</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>63453</v>
+        <v>10040</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>19603</v>
+        <v>64227</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>15066</v>
+        <v>54923</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>10296</v>
+        <v>27424</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>55608</v>
+        <v>81882</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>21279</v>
+        <v>92228</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>70605</v>
+        <v>86825</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" ca="1" si="0"/>
-        <v>65168</v>
+        <v>93540</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ca="1" si="0"/>
-        <v>69252</v>
+        <v>14903</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ca="1" si="0"/>
-        <v>66717</v>
+        <v>94876</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" ca="1" si="0"/>
-        <v>56973</v>
+        <v>31676</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" ca="1" si="0"/>
-        <v>71581</v>
+        <v>38816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DC0507-2589-4AC1-9862-D7928C83B4FC}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>32439</v>
+      </c>
+      <c r="B2">
+        <v>82597</v>
+      </c>
+      <c r="C2">
+        <v>65945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>95932</v>
+      </c>
+      <c r="B3">
+        <v>49302</v>
+      </c>
+      <c r="C3">
+        <v>60654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16825</v>
+      </c>
+      <c r="B4">
+        <v>23778</v>
+      </c>
+      <c r="C4">
+        <v>49267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>89310</v>
+      </c>
+      <c r="B5">
+        <v>58914</v>
+      </c>
+      <c r="C5">
+        <v>75811</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>59468</v>
+      </c>
+      <c r="C6">
+        <v>30613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>57913</v>
+      </c>
+      <c r="C7">
+        <v>98622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>80324</v>
+      </c>
+      <c r="C8">
+        <v>12011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>63892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>79388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>49051</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>66863</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>45446</v>
       </c>
     </row>
   </sheetData>
@@ -1181,282 +1173,117 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DC0507-2589-4AC1-9862-D7928C83B4FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213BADF4-84EF-4347-B750-C4FDA302935A}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f ca="1">RANDBETWEEN(10000,99999)</f>
-        <v>47017</v>
+        <v>69474</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="A2:D13" ca="1" si="0">RANDBETWEEN(10000,99999)</f>
-        <v>52585</v>
+        <v>73340</v>
       </c>
       <c r="C2">
-        <f t="shared" ca="1" si="0"/>
-        <v>40692</v>
+        <v>61771</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ca="1" si="0"/>
-        <v>28953</v>
+        <v>58484</v>
       </c>
       <c r="B3">
-        <f t="shared" ca="1" si="0"/>
-        <v>26682</v>
+        <v>41637</v>
       </c>
       <c r="C3">
-        <f t="shared" ca="1" si="0"/>
-        <v>41449</v>
+        <v>38036</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ca="1" si="0"/>
-        <v>50228</v>
+        <v>94786</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>60962</v>
+        <v>72544</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>48668</v>
+        <v>26484</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>81045</v>
+        <v>74713</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>56796</v>
+        <v>60357</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>26988</v>
+        <v>18310</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>59330</v>
+        <v>83167</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>16757</v>
+        <v>58019</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>76198</v>
+        <v>62260</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>19933</v>
+        <v>17681</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>52898</v>
+        <v>81086</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>19022</v>
+        <v>25046</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" ca="1" si="0"/>
-        <v>56839</v>
+        <v>18873</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ca="1" si="0"/>
-        <v>14838</v>
+        <v>93430</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ca="1" si="0"/>
-        <v>30317</v>
+        <v>95309</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" ca="1" si="0"/>
-        <v>84923</v>
+        <v>41218</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" ca="1" si="0"/>
-        <v>21010</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213BADF4-84EF-4347-B750-C4FDA302935A}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f ca="1">RANDBETWEEN(10000,99999)</f>
-        <v>11192</v>
-      </c>
-      <c r="B2">
-        <f t="shared" ref="A2:D13" ca="1" si="0">RANDBETWEEN(10000,99999)</f>
-        <v>33531</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ca="1" si="0"/>
-        <v>32337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ca="1" si="0"/>
-        <v>35796</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ca="1" si="0"/>
-        <v>83056</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ca="1" si="0"/>
-        <v>70503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" ca="1" si="0"/>
-        <v>32911</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>70486</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>66188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>89239</v>
-      </c>
-      <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>33323</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>72907</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>91386</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>98747</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>14283</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>50360</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>49099</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" ca="1" si="0"/>
-        <v>82951</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" ca="1" si="0"/>
-        <v>76748</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" ca="1" si="0"/>
-        <v>43793</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" ca="1" si="0"/>
-        <v>81329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" ca="1" si="0"/>
-        <v>31460</v>
+        <v>75835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improving data clean script to act as a function
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B00994-A718-4C12-BD3E-2A4F811DFE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34899389-7C86-472F-BF0E-B08B93534EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="19090" yWindow="2400" windowWidth="19420" windowHeight="10420" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
-    <sheet name="markers" sheetId="1" r:id="rId1"/>
-    <sheet name="paints" sheetId="4" r:id="rId2"/>
-    <sheet name="personal" sheetId="5" r:id="rId3"/>
-    <sheet name="private" sheetId="9" r:id="rId4"/>
-    <sheet name="business1" sheetId="6" r:id="rId5"/>
-    <sheet name="business2" sheetId="8" r:id="rId6"/>
-    <sheet name="business3" sheetId="7" r:id="rId7"/>
+    <sheet name="watercolours" sheetId="10" r:id="rId1"/>
+    <sheet name="markers" sheetId="1" r:id="rId2"/>
+    <sheet name="paints" sheetId="4" r:id="rId3"/>
+    <sheet name="personal" sheetId="5" r:id="rId4"/>
+    <sheet name="private" sheetId="9" r:id="rId5"/>
+    <sheet name="business1" sheetId="6" r:id="rId6"/>
+    <sheet name="business2" sheetId="8" r:id="rId7"/>
+    <sheet name="business3" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
   <si>
     <t>Blue</t>
   </si>
@@ -249,6 +250,42 @@
   </si>
   <si>
     <t>red01 p</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Pastel Pink^</t>
+  </si>
+  <si>
+    <t>Royal Purple</t>
+  </si>
+  <si>
+    <t>Sea Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rose Pink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Eggplant Purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azure Blue      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very   Pink   </t>
+  </si>
+  <si>
+    <t>Velvet Purple%$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg Blue       </t>
+  </si>
+  <si>
+    <t>Rouge Pink</t>
+  </si>
+  <si>
+    <t>Baby Pink</t>
   </si>
 </sst>
 </file>
@@ -605,6 +642,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8D6783-708B-4302-9BA2-BB2FDAA48E21}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECF79E4-6714-4A79-A3C9-5B59CFD0CFFC}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -687,11 +801,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8021D7E5-C5D3-468A-8962-5308880DA2DD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -750,7 +864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8200B3D-79D9-4DB0-A7F2-3CBE4D435429}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -851,7 +965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B705373B-808D-4771-B708-A48EFE188BCB}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -934,7 +1048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5A2C93-BD89-4B55-941F-F99B73CD3264}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1053,7 +1167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DC0507-2589-4AC1-9862-D7928C83B4FC}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1172,7 +1286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213BADF4-84EF-4347-B750-C4FDA302935A}">
   <dimension ref="A1:C13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updating colour_roll to accommodate match and mix selection settings
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34899389-7C86-472F-BF0E-B08B93534EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE2E546-9765-45FF-8670-567F6A48A4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="2400" windowWidth="19420" windowHeight="10420" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="watercolours" sheetId="10" r:id="rId1"/>
-    <sheet name="markers" sheetId="1" r:id="rId2"/>
-    <sheet name="paints" sheetId="4" r:id="rId3"/>
-    <sheet name="personal" sheetId="5" r:id="rId4"/>
-    <sheet name="private" sheetId="9" r:id="rId5"/>
-    <sheet name="business1" sheetId="6" r:id="rId6"/>
-    <sheet name="business2" sheetId="8" r:id="rId7"/>
-    <sheet name="business3" sheetId="7" r:id="rId8"/>
+    <sheet name="crayons" sheetId="11" r:id="rId2"/>
+    <sheet name="markers" sheetId="1" r:id="rId3"/>
+    <sheet name="paints" sheetId="4" r:id="rId4"/>
+    <sheet name="personal" sheetId="5" r:id="rId5"/>
+    <sheet name="private" sheetId="9" r:id="rId6"/>
+    <sheet name="business1" sheetId="6" r:id="rId7"/>
+    <sheet name="business2" sheetId="8" r:id="rId8"/>
+    <sheet name="business3" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t>Blue</t>
   </si>
@@ -286,6 +287,30 @@
   </si>
   <si>
     <t>Baby Pink</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indigo  </t>
+  </si>
+  <si>
+    <t>*Violet**]</t>
+  </si>
+  <si>
+    <t>bl^ue</t>
   </si>
 </sst>
 </file>
@@ -645,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8D6783-708B-4302-9BA2-BB2FDAA48E21}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,6 +744,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68ADE2F-BBDE-4953-B524-72AB78AABB7F}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECF79E4-6714-4A79-A3C9-5B59CFD0CFFC}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -801,7 +884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8021D7E5-C5D3-468A-8962-5308880DA2DD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -864,7 +947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8200B3D-79D9-4DB0-A7F2-3CBE4D435429}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -965,7 +1048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B705373B-808D-4771-B708-A48EFE188BCB}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1048,7 +1131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5A2C93-BD89-4B55-941F-F99B73CD3264}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1167,7 +1250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DC0507-2589-4AC1-9862-D7928C83B4FC}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1286,7 +1369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213BADF4-84EF-4347-B750-C4FDA302935A}">
   <dimension ref="A1:C13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding 'single' option to colour roller
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bjss-my.sharepoint.com/personal/amy_otway_bjss_com/Documents/Scripts/PycharmProjects/ColourRoller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{BEE2E546-9765-45FF-8670-567F6A48A4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0683302-F93D-47A2-A595-B7188D318A5B}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{BEE2E546-9765-45FF-8670-567F6A48A4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4015CAA8-8E2A-4BCA-93ED-2EFAB4BB4F48}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="watercolours" sheetId="10" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="business1" sheetId="6" r:id="rId7"/>
     <sheet name="business2" sheetId="8" r:id="rId8"/>
     <sheet name="business3" sheetId="7" r:id="rId9"/>
+    <sheet name="test" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
   <si>
     <t>Blue</t>
   </si>
@@ -347,6 +348,42 @@
   </si>
   <si>
     <t>Neon* *Pink</t>
+  </si>
+  <si>
+    <t>pens</t>
+  </si>
+  <si>
+    <t>pencils</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>indigo</t>
+  </si>
+  <si>
+    <t>violet</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>blender</t>
   </si>
 </sst>
 </file>
@@ -405,6 +442,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -706,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8D6783-708B-4302-9BA2-BB2FDAA48E21}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -832,6 +873,76 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155EC8E4-369A-4026-8FC5-5445D0909DD3}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added de-duplication functionality to data_clean
</commit_message>
<xml_diff>
--- a/colours2.xlsx
+++ b/colours2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bjss-my.sharepoint.com/personal/amy_otway_bjss_com/Documents/Scripts/PycharmProjects/ColourRoller/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy.Otway\OneDrive - BJSS Ltd\Scripts\PycharmProjects\ColourRoller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{BEE2E546-9765-45FF-8670-567F6A48A4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4015CAA8-8E2A-4BCA-93ED-2EFAB4BB4F48}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C218D6BC-0140-4B86-8F18-4B49CE3B924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18BCDF73-7175-4ABC-9973-74FD93318876}"/>
   </bookViews>
   <sheets>
     <sheet name="watercolours" sheetId="10" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="115">
   <si>
     <t>Blue</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>blender</t>
+  </si>
+  <si>
+    <t>Royal Purple&amp;</t>
+  </si>
+  <si>
+    <t>Eggplant~ Purple</t>
   </si>
 </sst>
 </file>
@@ -444,14 +450,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -489,7 +491,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -595,7 +597,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -737,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -745,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8D6783-708B-4302-9BA2-BB2FDAA48E21}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +776,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
@@ -796,7 +798,7 @@
         <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
         <v>78</v>
@@ -807,13 +809,16 @@
         <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -825,53 +830,53 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>100</v>
       </c>
     </row>
@@ -884,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155EC8E4-369A-4026-8FC5-5445D0909DD3}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>

</xml_diff>